<commit_message>
EL BOM cost report update
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
+++ b/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\STUF2019\CR - Cost Report\BOM\EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B2006F-BA7D-4A6F-88B2-F8C3C27FD3FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB95BF82-A082-4222-94E1-1FB22CDEBF67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="2610" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4590" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="258">
   <si>
     <t>System</t>
   </si>
@@ -64,16 +64,7 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name of the part</t>
-  </si>
-  <si>
-    <t>m or b</t>
-  </si>
-  <si>
     <t>Short description of the part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number </t>
   </si>
   <si>
     <r>
@@ -190,9 +181,6 @@
     <t>EL_05001</t>
   </si>
   <si>
-    <t>EL_05002</t>
-  </si>
-  <si>
     <t>EL_05003</t>
   </si>
   <si>
@@ -223,9 +211,6 @@
     <t>EL_06005</t>
   </si>
   <si>
-    <t>EL_06006</t>
-  </si>
-  <si>
     <t>EL_A0007</t>
   </si>
   <si>
@@ -328,15 +313,6 @@
     <t>EL_01012</t>
   </si>
   <si>
-    <t>dashboard supports upper</t>
-  </si>
-  <si>
-    <t>dashboard supports lower</t>
-  </si>
-  <si>
-    <t>crash sensor</t>
-  </si>
-  <si>
     <t>ride hand side of the front hoop</t>
   </si>
   <si>
@@ -358,9 +334,6 @@
     <t>Fuel pressure sensor</t>
   </si>
   <si>
-    <t>brake pedal contact</t>
-  </si>
-  <si>
     <t>front harness</t>
   </si>
   <si>
@@ -412,9 +385,6 @@
     <t>EL_02007</t>
   </si>
   <si>
-    <t>EL_02008</t>
-  </si>
-  <si>
     <t>EL_02009</t>
   </si>
   <si>
@@ -688,18 +658,9 @@
     <t>EL_05009</t>
   </si>
   <si>
-    <t>main hoop kill Switch</t>
-  </si>
-  <si>
     <t>Dashboard kill Switch</t>
   </si>
   <si>
-    <t>Brake kill Switch</t>
-  </si>
-  <si>
-    <t>inertia switch</t>
-  </si>
-  <si>
     <t>Master switch</t>
   </si>
   <si>
@@ -707,13 +668,175 @@
   </si>
   <si>
     <t>folded aluminium ?</t>
+  </si>
+  <si>
+    <t>front board</t>
+  </si>
+  <si>
+    <t>front board box</t>
+  </si>
+  <si>
+    <t>EL_02022</t>
+  </si>
+  <si>
+    <t>EL_02023</t>
+  </si>
+  <si>
+    <t>3 phase rectifier</t>
+  </si>
+  <si>
+    <t>BSPD</t>
+  </si>
+  <si>
+    <t>BOTS</t>
+  </si>
+  <si>
+    <t>data logger</t>
+  </si>
+  <si>
+    <t>MK3</t>
+  </si>
+  <si>
+    <t>Brake light</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t>data log connector set</t>
+  </si>
+  <si>
+    <t>ECU connector set</t>
+  </si>
+  <si>
+    <t>Servo motor</t>
+  </si>
+  <si>
+    <t>Servo motor cables</t>
+  </si>
+  <si>
+    <t>Rear board shifter</t>
+  </si>
+  <si>
+    <t>Rear box shifter</t>
+  </si>
+  <si>
+    <t>Main hoop kill Switch</t>
+  </si>
+  <si>
+    <t>Crash sensor</t>
+  </si>
+  <si>
+    <t>servo motor support</t>
+  </si>
+  <si>
+    <t>starter relay</t>
+  </si>
+  <si>
+    <t>EL_05010</t>
+  </si>
+  <si>
+    <t>EL_05011</t>
+  </si>
+  <si>
+    <t>EL_05012</t>
+  </si>
+  <si>
+    <t>EL_05013</t>
+  </si>
+  <si>
+    <t>EL_05014</t>
+  </si>
+  <si>
+    <t>EL_04007</t>
+  </si>
+  <si>
+    <t>mounted on the fire wall</t>
+  </si>
+  <si>
+    <t>RPM display</t>
+  </si>
+  <si>
+    <t>standard emergency button</t>
+  </si>
+  <si>
+    <t>contact switch</t>
+  </si>
+  <si>
+    <t>for secondary fonctions</t>
+  </si>
+  <si>
+    <t>display engaged gear</t>
+  </si>
+  <si>
+    <t>display water temp. Or Batt. Voltage</t>
+  </si>
+  <si>
+    <t>control for the Dashboard and sensors</t>
+  </si>
+  <si>
+    <t>connector for MK3</t>
+  </si>
+  <si>
+    <t>to the DTA</t>
+  </si>
+  <si>
+    <t>to the MK3</t>
+  </si>
+  <si>
+    <t>rear red light</t>
+  </si>
+  <si>
+    <t>connector set for the DTA</t>
+  </si>
+  <si>
+    <t>DTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12V </t>
+  </si>
+  <si>
+    <t>fan relay 35A</t>
+  </si>
+  <si>
+    <t>Pump relay 35A</t>
+  </si>
+  <si>
+    <t>DTA Power relay 35A</t>
+  </si>
+  <si>
+    <t>rear board relay 35A</t>
+  </si>
+  <si>
+    <t>inside the fuse box</t>
+  </si>
+  <si>
+    <t>change the gears</t>
+  </si>
+  <si>
+    <t>on both sides of the main hoop</t>
+  </si>
+  <si>
+    <t>on the Dashboard</t>
+  </si>
+  <si>
+    <t>behind the brake pedale</t>
+  </si>
+  <si>
+    <t>ride hand side of the front hoop ?</t>
+  </si>
+  <si>
+    <t>protecting plastic case</t>
+  </si>
+  <si>
+    <t>controled high power motor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -758,13 +881,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -835,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -850,9 +966,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1135,11 +1248,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1179,1611 +1292,1724 @@
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>232</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>8</v>
+        <v>233</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>8</v>
+        <v>235</v>
       </c>
       <c r="F6" s="3">
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>234</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="F9" s="3">
         <v>2</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>236</v>
+      </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>237</v>
+      </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="5" t="s">
-        <v>90</v>
+      <c r="C13" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>238</v>
+      </c>
       <c r="F13" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="5" t="s">
-        <v>91</v>
+      <c r="C14" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>256</v>
+      </c>
       <c r="F14" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>92</v>
+        <v>211</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>93</v>
+        <v>212</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>94</v>
+        <v>215</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>93</v>
+        <v>239</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="F18" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F19" s="3">
         <v>4</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="F20" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="F21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="6" t="s">
-        <v>100</v>
+      <c r="C22" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="F22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>240</v>
+      </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>240</v>
+      </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>240</v>
+      </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>139</v>
+        <v>240</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
-        <v>111</v>
+      <c r="C32" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="3" t="s">
-        <v>104</v>
+      <c r="F33" s="3">
+        <v>4</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="F34" s="3">
         <v>4</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="F35" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="5" t="s">
-        <v>116</v>
+      <c r="C36" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="F36" s="3">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>131</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4" t="s">
-        <v>28</v>
+      <c r="C37" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" s="3">
+        <v>22</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="F41" s="3">
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F42" s="3">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F43" s="3">
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F44" s="3">
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F47" s="3">
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F48" s="3">
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F49" s="3">
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F50" s="3">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F51" s="3">
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F52" s="3">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F53" s="3">
         <v>1</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F54" s="3">
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="F55" s="3">
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="F56" s="3">
         <v>1</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F57" s="3">
-        <v>1</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="F57" s="3"/>
       <c r="G57" s="3" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>156</v>
+        <v>214</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F58" s="3">
-        <v>22</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="F58" s="3"/>
       <c r="G58" s="3" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F59" s="3">
-        <v>22</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="F59" s="3"/>
       <c r="G59" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3">
-        <v>2</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4" t="s">
-        <v>29</v>
+      <c r="E61" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F61" s="3">
+        <v>1</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
-        <v>191</v>
+        <v>59</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>216</v>
+        <v>67</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="F62" s="3">
         <v>1</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>64</v>
+        <v>182</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E63" s="3"/>
       <c r="F63" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1</v>
+      </c>
       <c r="G64" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
       <c r="G65" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
+      <c r="F66" s="3">
+        <v>1</v>
+      </c>
       <c r="G66" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
       <c r="G67" s="3" t="s">
-        <v>41</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="F69" s="3">
         <v>1</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F70" s="3">
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F71" s="3">
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>202</v>
+        <v>6</v>
       </c>
       <c r="F72" s="3">
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="F73" s="3">
         <v>1</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1</v>
+      </c>
+      <c r="G74" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="F74" s="3">
-        <v>1</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1</v>
+      </c>
+      <c r="G75" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="F75" s="3">
-        <v>1</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>205</v>
+        <v>251</v>
       </c>
       <c r="F76" s="3">
         <v>1</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E77" s="3"/>
       <c r="F77" s="3">
         <v>1</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4" t="s">
-        <v>49</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3" t="s">
-        <v>210</v>
+        <v>247</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>8</v>
+        <v>250</v>
       </c>
       <c r="F79" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>50</v>
+        <v>227</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>8</v>
+        <v>250</v>
       </c>
       <c r="F80" s="3">
         <v>1</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>51</v>
+        <v>228</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3" t="s">
-        <v>212</v>
+        <v>249</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E81" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F81" s="3">
+        <v>1</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F81" s="3">
-        <v>1</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F82" s="3">
-        <v>1</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>53</v>
+      <c r="B82" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F83" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>8</v>
+        <v>253</v>
       </c>
       <c r="F84" s="3">
         <v>1</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F85" s="3">
+        <v>1</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>9</v>
+        <v>64</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E87" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F87" s="3">
+        <v>1</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>59</v>
+      <c r="B88" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3" t="s">
-        <v>6</v>
+        <v>220</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3">
+        <v>1</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3" t="s">
-        <v>6</v>
+        <v>219</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>9</v>
+        <v>256</v>
+      </c>
+      <c r="F90" s="3">
+        <v>1</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3" t="s">
-        <v>6</v>
+        <v>218</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3">
+        <v>1</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F92" s="3">
+        <v>1</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3">
+        <v>1</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F94" s="3">
+        <v>1</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C31 C1:C26 C78:C1048576 C39:C76" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30 C82:C1048576 C36:C75 C1:C26" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
       <formula1>25</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">

</xml_diff>

<commit_message>
CR EL : excel et premieres images
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
+++ b/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\STUF2019\CR - Cost Report\BOM\EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB95BF82-A082-4222-94E1-1FB22CDEBF67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AAE007-E9CB-44F9-8976-0AFFB5A3FDCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1785" yWindow="-285" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="256">
   <si>
     <t>System</t>
   </si>
@@ -280,12 +280,6 @@
     <t>push button</t>
   </si>
   <si>
-    <t>1 digit I2C display</t>
-  </si>
-  <si>
-    <t>3 digit I2C dislpay</t>
-  </si>
-  <si>
     <t>with a red light circle</t>
   </si>
   <si>
@@ -343,18 +337,6 @@
     <t>paddle</t>
   </si>
   <si>
-    <t>3?</t>
-  </si>
-  <si>
-    <t>wheel brake contact</t>
-  </si>
-  <si>
-    <t>Brake Temp sensor</t>
-  </si>
-  <si>
-    <t>Tyre temp sensor</t>
-  </si>
-  <si>
     <t>Oil pressure sensor</t>
   </si>
   <si>
@@ -418,12 +400,6 @@
     <t>EL_02019</t>
   </si>
   <si>
-    <t>EL_02020</t>
-  </si>
-  <si>
-    <t>EL_02021</t>
-  </si>
-  <si>
     <t>on each four suspensions</t>
   </si>
   <si>
@@ -667,21 +643,12 @@
     <t>Master switch pannel</t>
   </si>
   <si>
-    <t>folded aluminium ?</t>
-  </si>
-  <si>
     <t>front board</t>
   </si>
   <si>
     <t>front board box</t>
   </si>
   <si>
-    <t>EL_02022</t>
-  </si>
-  <si>
-    <t>EL_02023</t>
-  </si>
-  <si>
     <t>3 phase rectifier</t>
   </si>
   <si>
@@ -781,9 +748,6 @@
     <t>to the DTA</t>
   </si>
   <si>
-    <t>to the MK3</t>
-  </si>
-  <si>
     <t>rear red light</t>
   </si>
   <si>
@@ -793,9 +757,6 @@
     <t>DTA</t>
   </si>
   <si>
-    <t xml:space="preserve">12V </t>
-  </si>
-  <si>
     <t>fan relay 35A</t>
   </si>
   <si>
@@ -823,13 +784,46 @@
     <t>behind the brake pedale</t>
   </si>
   <si>
-    <t>ride hand side of the front hoop ?</t>
-  </si>
-  <si>
     <t>protecting plastic case</t>
   </si>
   <si>
     <t>controled high power motor</t>
+  </si>
+  <si>
+    <t>right hand side of the front hoop</t>
+  </si>
+  <si>
+    <t>1 digit I2C display board</t>
+  </si>
+  <si>
+    <t>3 digit I2C dislpay board</t>
+  </si>
+  <si>
+    <t>in the steering rack</t>
+  </si>
+  <si>
+    <t>EL_02008</t>
+  </si>
+  <si>
+    <t>folded aluminium</t>
+  </si>
+  <si>
+    <t>12V Battery</t>
+  </si>
+  <si>
+    <t>standard battery connectors</t>
+  </si>
+  <si>
+    <t>on the right hand side of the main hoop</t>
+  </si>
+  <si>
+    <t>on the right hand side of the motor</t>
+  </si>
+  <si>
+    <t>set of cable for the servo motor</t>
+  </si>
+  <si>
+    <t>made in steel</t>
   </si>
 </sst>
 </file>
@@ -1248,11 +1242,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F91" sqref="F91"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1328,7 @@
         <v>67</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -1353,7 +1347,7 @@
         <v>67</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1372,7 +1366,7 @@
         <v>67</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F6" s="3">
         <v>4</v>
@@ -1391,7 +1385,7 @@
         <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
@@ -1410,7 +1404,7 @@
         <v>67</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -1429,13 +1423,13 @@
         <v>67</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F9" s="3">
         <v>2</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1448,89 +1442,89 @@
         <v>67</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="5" t="s">
-        <v>74</v>
+      <c r="C11" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="5" t="s">
-        <v>75</v>
+      <c r="C12" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1552,13 +1546,13 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1571,13 +1565,13 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -1590,13 +1584,13 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -1609,13 +1603,13 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F19" s="3">
         <v>4</v>
@@ -1628,13 +1622,13 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F20" s="3">
         <v>4</v>
@@ -1647,13 +1641,13 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
@@ -1666,1350 +1660,1307 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F22" s="3">
         <v>2</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>109</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="5" t="s">
-        <v>98</v>
+      <c r="C32" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>95</v>
+        <v>119</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="5" t="s">
-        <v>96</v>
+      <c r="C33" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="F33" s="3">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="5" t="s">
-        <v>97</v>
+      <c r="C34" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>241</v>
+        <v>144</v>
       </c>
       <c r="F34" s="3">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>146</v>
+        <v>90</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="F36" s="3">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>206</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="F37" s="3">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F41" s="3">
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="F42" s="3">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F43" s="3">
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F44" s="3">
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F47" s="3">
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F48" s="3">
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F49" s="3">
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F50" s="3">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F51" s="3">
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="F52" s="3">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="F53" s="3">
         <v>1</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>141</v>
+        <v>202</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F54" s="3">
-        <v>1</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F55" s="3">
-        <v>1</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="F55" s="3"/>
       <c r="G55" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F56" s="3">
-        <v>1</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="F56" s="3"/>
       <c r="G56" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F58" s="3"/>
+        <v>249</v>
+      </c>
+      <c r="F58" s="3">
+        <v>1</v>
+      </c>
       <c r="G58" s="3" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
-        <v>216</v>
+        <v>59</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="F59" s="3"/>
+        <v>250</v>
+      </c>
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
       <c r="G59" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F60" s="3">
+        <v>2</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>203</v>
+        <v>67</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F61" s="3">
         <v>1</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
-        <v>59</v>
+        <v>193</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="F62" s="3">
         <v>1</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E63" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>252</v>
+      </c>
       <c r="F63" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="F64" s="3">
         <v>1</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3">
-        <v>1</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>37</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E66" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="F66" s="3">
         <v>1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="F67" s="3">
         <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>190</v>
+        <v>6</v>
       </c>
       <c r="F69" s="3">
         <v>1</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F70" s="3">
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F71" s="3">
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>42</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="F72" s="3">
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>43</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>192</v>
+        <v>238</v>
       </c>
       <c r="F73" s="3">
         <v>1</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>44</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>192</v>
+        <v>253</v>
       </c>
       <c r="F74" s="3">
         <v>1</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3" t="s">
-        <v>196</v>
+        <v>233</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>195</v>
+        <v>237</v>
       </c>
       <c r="F75" s="3">
         <v>1</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>194</v>
+        <v>234</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="F76" s="3">
         <v>1</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E77" s="3"/>
+      <c r="E77" s="3" t="s">
+        <v>237</v>
+      </c>
       <c r="F77" s="3">
         <v>1</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="F78" s="3">
         <v>1</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="F79" s="3">
-        <v>1</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="F80" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>228</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F81" s="3">
         <v>1</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F82" s="3">
+        <v>1</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="F83" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="F84" s="3">
         <v>1</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F85" s="3">
-        <v>1</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
-      <c r="C86" s="3" t="s">
+      <c r="C86" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>255</v>
-      </c>
+      <c r="D86" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E86" s="5"/>
       <c r="F86" s="3">
         <v>1</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>85</v>
+        <v>242</v>
       </c>
       <c r="F87" s="3">
         <v>1</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F88" s="3">
+        <v>1</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E89" s="3"/>
+      <c r="E89" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="F89" s="3">
         <v>1</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
-      <c r="C90" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D90" s="3" t="s">
+      <c r="C90" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E90" s="3" t="s">
-        <v>256</v>
+      <c r="E90" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="F90" s="3">
         <v>1</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3" t="s">
-        <v>218</v>
+        <v>92</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="F91" s="3">
         <v>1</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F92" s="3">
-        <v>1</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3">
-        <v>1</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F94" s="3">
-        <v>1</v>
-      </c>
-      <c r="G94" s="3" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30 C82:C1048576 C36:C75 C1:C26" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30 C79:C1048576 C33:C72 C1:C26" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
       <formula1>25</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">

</xml_diff>

<commit_message>
EL BOM rename pictures
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
+++ b/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\STUF2019\CR - Cost Report\BOM\EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AAE007-E9CB-44F9-8976-0AFFB5A3FDCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A17684-CD58-4FE1-90E6-3B5BA8783E51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="-285" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="227">
   <si>
     <t>System</t>
   </si>
@@ -307,12 +307,6 @@
     <t>EL_01012</t>
   </si>
   <si>
-    <t>ride hand side of the front hoop</t>
-  </si>
-  <si>
-    <t>crash sensor's support</t>
-  </si>
-  <si>
     <t>wheel speed sensor</t>
   </si>
   <si>
@@ -397,9 +391,6 @@
     <t>EL_02018</t>
   </si>
   <si>
-    <t>EL_02019</t>
-  </si>
-  <si>
     <t>on each four suspensions</t>
   </si>
   <si>
@@ -442,36 +433,12 @@
     <t>connector rear board 2</t>
   </si>
   <si>
-    <t>connector servo motor 1</t>
-  </si>
-  <si>
-    <t>connector servo motor 2</t>
-  </si>
-  <si>
     <t>connector front board 1</t>
   </si>
   <si>
     <t>connector front board 2</t>
   </si>
   <si>
-    <t>connector Dashboard 1</t>
-  </si>
-  <si>
-    <t>connector Dashboard 2</t>
-  </si>
-  <si>
-    <t>connector front board 3</t>
-  </si>
-  <si>
-    <t>connector front board 4</t>
-  </si>
-  <si>
-    <t>connector BSPD 1</t>
-  </si>
-  <si>
-    <t>connector BSPD 2</t>
-  </si>
-  <si>
     <t>connector sensors</t>
   </si>
   <si>
@@ -481,48 +448,18 @@
     <t>8STA71828P, sensors and Power</t>
   </si>
   <si>
-    <t>8STA70835S, advance data logging</t>
-  </si>
-  <si>
-    <t>8STA70835P, advance data logging</t>
-  </si>
-  <si>
     <t>8STA10235S, to the harness (fr. or re.)</t>
   </si>
   <si>
     <t>8STA60235P, to the harness (fr. or re.)</t>
   </si>
   <si>
-    <t>8STA01035S, power and sensors</t>
-  </si>
-  <si>
-    <t>8STA61035P, power and sensors</t>
-  </si>
-  <si>
-    <t>8STA01497S, to the rear board</t>
-  </si>
-  <si>
-    <t>8STA61497P, to the rear board</t>
-  </si>
-  <si>
     <t>8STA01002S, 5V Power</t>
   </si>
   <si>
     <t>8STA61002P, 5V Power</t>
   </si>
   <si>
-    <t>8STA00435S, Data Bus</t>
-  </si>
-  <si>
-    <t>8STA60435P, Data Bus</t>
-  </si>
-  <si>
-    <t>8STA01035S, Power and data</t>
-  </si>
-  <si>
-    <t>8STA61035P, Power and data</t>
-  </si>
-  <si>
     <t>8STA01497PB, Power and DATA</t>
   </si>
   <si>
@@ -550,27 +487,6 @@
     <t>EL_03013</t>
   </si>
   <si>
-    <t>EL_03014</t>
-  </si>
-  <si>
-    <t>EL_03015</t>
-  </si>
-  <si>
-    <t>EL_03016</t>
-  </si>
-  <si>
-    <t>EL_03017</t>
-  </si>
-  <si>
-    <t>EL_03018</t>
-  </si>
-  <si>
-    <t>EL_03019</t>
-  </si>
-  <si>
-    <t>EL_03020</t>
-  </si>
-  <si>
     <t>link fr. , servo motor, sensors, bat.</t>
   </si>
   <si>
@@ -583,9 +499,6 @@
     <t>Battery connector</t>
   </si>
   <si>
-    <t>EL_03021</t>
-  </si>
-  <si>
     <t>Battery Fuse 250A</t>
   </si>
   <si>
@@ -706,15 +619,6 @@
     <t>EL_05011</t>
   </si>
   <si>
-    <t>EL_05012</t>
-  </si>
-  <si>
-    <t>EL_05013</t>
-  </si>
-  <si>
-    <t>EL_05014</t>
-  </si>
-  <si>
     <t>EL_04007</t>
   </si>
   <si>
@@ -757,21 +661,6 @@
     <t>DTA</t>
   </si>
   <si>
-    <t>fan relay 35A</t>
-  </si>
-  <si>
-    <t>Pump relay 35A</t>
-  </si>
-  <si>
-    <t>DTA Power relay 35A</t>
-  </si>
-  <si>
-    <t>rear board relay 35A</t>
-  </si>
-  <si>
-    <t>inside the fuse box</t>
-  </si>
-  <si>
     <t>change the gears</t>
   </si>
   <si>
@@ -805,9 +694,6 @@
     <t>EL_02008</t>
   </si>
   <si>
-    <t>folded aluminium</t>
-  </si>
-  <si>
     <t>12V Battery</t>
   </si>
   <si>
@@ -824,6 +710,33 @@
   </si>
   <si>
     <t>made in steel</t>
+  </si>
+  <si>
+    <t>Picture/drawing</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>relays 35A</t>
+  </si>
+  <si>
+    <t>in the fuse box, fan, pump, DTA, rear</t>
+  </si>
+  <si>
+    <t>on the rear rigth side</t>
+  </si>
+  <si>
+    <t>Booster</t>
+  </si>
+  <si>
+    <t>EL_04008</t>
+  </si>
+  <si>
+    <t>8STA70835S, Power and DATA</t>
+  </si>
+  <si>
+    <t>8STA70835P,Power and DATA</t>
   </si>
 </sst>
 </file>
@@ -945,7 +858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -961,6 +874,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1242,11 +1164,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,10 +1180,10 @@
     <col min="5" max="5" width="45.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1283,8 +1205,11 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1299,7 +1224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -1318,7 +1243,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
@@ -1328,7 +1253,7 @@
         <v>67</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -1336,8 +1261,11 @@
       <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
@@ -1347,7 +1275,7 @@
         <v>67</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1355,8 +1283,11 @@
       <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -1366,7 +1297,7 @@
         <v>67</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="F6" s="3">
         <v>4</v>
@@ -1374,8 +1305,11 @@
       <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -1385,7 +1319,7 @@
         <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
@@ -1393,8 +1327,11 @@
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
@@ -1412,8 +1349,11 @@
       <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
@@ -1431,8 +1371,11 @@
       <c r="G9" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
@@ -1450,18 +1393,21 @@
       <c r="G10" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -1469,18 +1415,21 @@
       <c r="G11" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
@@ -1488,18 +1437,21 @@
       <c r="G12" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -1508,17 +1460,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -1526,8 +1478,11 @@
       <c r="G14" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -1542,36 +1497,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -1584,16 +1542,16 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="F18" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>21</v>
@@ -1603,13 +1561,13 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F19" s="3">
         <v>4</v>
@@ -1622,16 +1580,16 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>114</v>
+        <v>210</v>
       </c>
       <c r="F20" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>23</v>
@@ -1641,16 +1599,16 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>247</v>
+        <v>113</v>
       </c>
       <c r="F21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>24</v>
@@ -1660,57 +1618,57 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F22" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1723,297 +1681,297 @@
         <v>67</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>120</v>
+        <v>197</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>229</v>
+        <v>115</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>118</v>
+        <v>197</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>229</v>
+        <v>116</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="F32" s="3">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F33" s="3">
         <v>22</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F34" s="3">
-        <v>22</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>140</v>
+        <v>225</v>
       </c>
       <c r="F39" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>141</v>
+        <v>226</v>
       </c>
       <c r="F40" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
@@ -2023,944 +1981,768 @@
         <v>67</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="F42" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="F43" s="3">
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="F44" s="3">
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>148</v>
+        <v>198</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="F47" s="3">
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="F49" s="3">
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>153</v>
+        <v>212</v>
       </c>
       <c r="F50" s="3">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="F51" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="F52" s="3">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
       <c r="F53" s="3">
         <v>1</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F54" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="F54" s="3">
+        <v>1</v>
+      </c>
       <c r="G54" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="F55" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
       <c r="G55" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="F56" s="3"/>
+        <v>188</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
       <c r="G56" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>249</v>
+        <v>153</v>
       </c>
       <c r="F58" s="3">
         <v>1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>250</v>
+        <v>155</v>
       </c>
       <c r="F59" s="3">
         <v>1</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>251</v>
+        <v>155</v>
       </c>
       <c r="F60" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>183</v>
+        <v>6</v>
       </c>
       <c r="F61" s="3">
         <v>1</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>252</v>
+        <v>155</v>
       </c>
       <c r="F62" s="3">
         <v>1</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>252</v>
+        <v>155</v>
       </c>
       <c r="F63" s="3">
         <v>1</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>220</v>
+        <v>158</v>
       </c>
       <c r="F64" s="3">
         <v>1</v>
       </c>
       <c r="G64" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H65" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="F66" s="3">
         <v>1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>184</v>
+        <v>221</v>
       </c>
       <c r="F67" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F68" s="3">
-        <v>1</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>6</v>
+        <v>202</v>
       </c>
       <c r="F69" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="F70" s="3">
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="F71" s="3">
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="F72" s="3">
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="F73" s="3">
         <v>1</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F74" s="3">
-        <v>1</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
-      <c r="C75" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>237</v>
-      </c>
+      <c r="C75" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E75" s="5"/>
       <c r="F75" s="3">
         <v>1</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>234</v>
+        <v>179</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="F76" s="3">
         <v>1</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3" t="s">
-        <v>235</v>
+        <v>178</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="F77" s="3">
         <v>1</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3" t="s">
-        <v>236</v>
+        <v>177</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="F78" s="3">
         <v>1</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F79" s="3">
+        <v>1</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3" t="s">
-        <v>210</v>
+        <v>90</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>239</v>
+        <v>118</v>
       </c>
       <c r="F80" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F81" s="3">
-        <v>1</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F82" s="3">
-        <v>1</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F83" s="3">
-        <v>1</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F84" s="3">
-        <v>1</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E86" s="5"/>
-      <c r="F86" s="3">
-        <v>1</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F87" s="3">
-        <v>1</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F88" s="3">
-        <v>1</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="F89" s="3">
-        <v>1</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="F90" s="3">
-        <v>1</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F91" s="3">
-        <v>1</v>
-      </c>
-      <c r="G91" s="3" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30 C79:C1048576 C33:C72 C1:C26" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C29 C68:C1048576 C1:C25 C32:C64" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
       <formula1>25</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">

</xml_diff>

<commit_message>
Update EL BOM plus d'image
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
+++ b/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\STUF2019\CR - Cost Report\BOM\EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A17684-CD58-4FE1-90E6-3B5BA8783E51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD993B1-5E57-4174-A15F-8F0F9601E334}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8940" yWindow="660" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="214">
   <si>
     <t>System</t>
   </si>
@@ -64,9 +64,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Short description of the part</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Part </t>
     </r>
@@ -100,9 +97,6 @@
     <t>EL_01002</t>
   </si>
   <si>
-    <t>EL_01003</t>
-  </si>
-  <si>
     <t>EL_01004</t>
   </si>
   <si>
@@ -262,9 +256,6 @@
     <t>b</t>
   </si>
   <si>
-    <t>Emergency Stop button</t>
-  </si>
-  <si>
     <t>2 way switch</t>
   </si>
   <si>
@@ -388,9 +379,6 @@
     <t>EL_02017</t>
   </si>
   <si>
-    <t>EL_02018</t>
-  </si>
-  <si>
     <t>on each four suspensions</t>
   </si>
   <si>
@@ -418,15 +406,9 @@
     <t xml:space="preserve">connector data log 1 </t>
   </si>
   <si>
-    <t>connector data log 2</t>
-  </si>
-  <si>
     <t>connector front-rear 1</t>
   </si>
   <si>
-    <t>connector front-rear 2</t>
-  </si>
-  <si>
     <t>connector rear board 1</t>
   </si>
   <si>
@@ -436,36 +418,9 @@
     <t>connector front board 1</t>
   </si>
   <si>
-    <t>connector front board 2</t>
-  </si>
-  <si>
     <t>connector sensors</t>
   </si>
   <si>
-    <t>8STA71828S, sensors and Power</t>
-  </si>
-  <si>
-    <t>8STA71828P, sensors and Power</t>
-  </si>
-  <si>
-    <t>8STA10235S, to the harness (fr. or re.)</t>
-  </si>
-  <si>
-    <t>8STA60235P, to the harness (fr. or re.)</t>
-  </si>
-  <si>
-    <t>8STA01002S, 5V Power</t>
-  </si>
-  <si>
-    <t>8STA61002P, 5V Power</t>
-  </si>
-  <si>
-    <t>8STA01497PB, Power and DATA</t>
-  </si>
-  <si>
-    <t>8STA61497SB, Power and DATA</t>
-  </si>
-  <si>
     <t>EL_03007</t>
   </si>
   <si>
@@ -481,12 +436,6 @@
     <t>EL_03011</t>
   </si>
   <si>
-    <t>EL_03012</t>
-  </si>
-  <si>
-    <t>EL_03013</t>
-  </si>
-  <si>
     <t>link fr. , servo motor, sensors, bat.</t>
   </si>
   <si>
@@ -502,18 +451,12 @@
     <t>Battery Fuse 250A</t>
   </si>
   <si>
-    <t>Fan Fuse 10A</t>
-  </si>
-  <si>
     <t>Lambda sensor Fuse 5A</t>
   </si>
   <si>
     <t>Pump Fuse 20A</t>
   </si>
   <si>
-    <t>Injection Fuse 10A</t>
-  </si>
-  <si>
     <t>Rear Fuse Box</t>
   </si>
   <si>
@@ -529,24 +472,12 @@
     <t>Brake light Fuse 2A</t>
   </si>
   <si>
-    <t>Servo motor 15A</t>
-  </si>
-  <si>
-    <t>Front board and data Logger</t>
-  </si>
-  <si>
-    <t>Front harness Fuse 10A</t>
-  </si>
-  <si>
     <t>EL_05007</t>
   </si>
   <si>
     <t>EL_05008</t>
   </si>
   <si>
-    <t>EL_05009</t>
-  </si>
-  <si>
     <t>Dashboard kill Switch</t>
   </si>
   <si>
@@ -613,12 +544,6 @@
     <t>starter relay</t>
   </si>
   <si>
-    <t>EL_05010</t>
-  </si>
-  <si>
-    <t>EL_05011</t>
-  </si>
-  <si>
     <t>EL_04007</t>
   </si>
   <si>
@@ -628,9 +553,6 @@
     <t>RPM display</t>
   </si>
   <si>
-    <t>standard emergency button</t>
-  </si>
-  <si>
     <t>contact switch</t>
   </si>
   <si>
@@ -643,9 +565,6 @@
     <t>display water temp. Or Batt. Voltage</t>
   </si>
   <si>
-    <t>control for the Dashboard and sensors</t>
-  </si>
-  <si>
     <t>connector for MK3</t>
   </si>
   <si>
@@ -661,9 +580,6 @@
     <t>DTA</t>
   </si>
   <si>
-    <t>change the gears</t>
-  </si>
-  <si>
     <t>on both sides of the main hoop</t>
   </si>
   <si>
@@ -697,9 +613,6 @@
     <t>12V Battery</t>
   </si>
   <si>
-    <t>standard battery connectors</t>
-  </si>
-  <si>
     <t>on the right hand side of the main hoop</t>
   </si>
   <si>
@@ -709,9 +622,6 @@
     <t>set of cable for the servo motor</t>
   </si>
   <si>
-    <t>made in steel</t>
-  </si>
-  <si>
     <t>Picture/drawing</t>
   </si>
   <si>
@@ -733,10 +643,61 @@
     <t>EL_04008</t>
   </si>
   <si>
-    <t>8STA70835S, Power and DATA</t>
-  </si>
-  <si>
-    <t>8STA70835P,Power and DATA</t>
+    <t>8STA01497P, Power and DATA</t>
+  </si>
+  <si>
+    <t>8STA61497S, Power and DATA</t>
+  </si>
+  <si>
+    <t>Servo motor Fuse 15A</t>
+  </si>
+  <si>
+    <t>change the gears, in the Fuse Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> in the Fuse box</t>
+  </si>
+  <si>
+    <t>battery connector</t>
+  </si>
+  <si>
+    <t>8STA10235S&amp;P, to the harness (fr./re.)</t>
+  </si>
+  <si>
+    <t>8STA71828S&amp;P, sensors and Power</t>
+  </si>
+  <si>
+    <t>8STA70835S&amp;P, Power and DATA</t>
+  </si>
+  <si>
+    <t>8STA01002S&amp;P, 5V Power</t>
+  </si>
+  <si>
+    <t>EL_05002</t>
+  </si>
+  <si>
+    <t>Fuse 10A</t>
+  </si>
+  <si>
+    <t>in the Fuse box, Fan, Inject., Fr. har.</t>
+  </si>
+  <si>
+    <t>DB-9 connector</t>
+  </si>
+  <si>
+    <t>Access to the DTA</t>
+  </si>
+  <si>
+    <t>control the servo motor</t>
+  </si>
+  <si>
+    <t>support the servo motor assembly</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>control the Dashboard and sensors</t>
   </si>
 </sst>
 </file>
@@ -1164,11 +1125,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1206,731 +1167,769 @@
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="F5" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>219</v>
+        <v>13</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="F6" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>219</v>
+        <v>14</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>191</v>
+        <v>71</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>219</v>
+        <v>15</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>219</v>
+        <v>73</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F9" s="3">
         <v>2</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>219</v>
+        <v>74</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>80</v>
+        <v>167</v>
       </c>
       <c r="F10" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>219</v>
+        <v>75</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>219</v>
+        <v>76</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>219</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
-        <v>18</v>
+        <v>79</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>175</v>
+        <v>80</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>196</v>
+        <v>108</v>
       </c>
       <c r="F17" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F18" s="3">
         <v>4</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="F19" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>210</v>
+        <v>109</v>
       </c>
       <c r="F20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>117</v>
+        <v>170</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>197</v>
+        <v>111</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>197</v>
+        <v>112</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>116</v>
+        <v>201</v>
       </c>
       <c r="F31" s="3">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F32" s="3">
-        <v>22</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>109</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="F33" s="3">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>27</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>143</v>
+        <v>203</v>
       </c>
       <c r="F36" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>128</v>
+        <v>195</v>
       </c>
       <c r="F37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>29</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>129</v>
+        <v>196</v>
       </c>
       <c r="F38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>30</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1940,300 +1939,326 @@
         <v>119</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="F39" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>31</v>
+        <v>121</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>226</v>
+        <v>171</v>
       </c>
       <c r="F40" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>32</v>
+        <v>122</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F41" s="3">
-        <v>2</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>136</v>
+      <c r="H41" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F42" s="3">
-        <v>2</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>137</v>
+      <c r="H42" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F43" s="3">
-        <v>1</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F44" s="3">
-        <v>1</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="H43" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>219</v>
+        <v>31</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>141</v>
+        <v>32</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F47" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4" t="s">
-        <v>26</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H48" s="3"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="F49" s="3">
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>219</v>
+        <v>35</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="F50" s="3">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>146</v>
+        <v>193</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="F51" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>35</v>
+        <v>162</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="F52" s="3">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F53" s="3">
-        <v>1</v>
-      </c>
-      <c r="G53" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H53" s="8" t="s">
-        <v>219</v>
-      </c>
+      <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>214</v>
+        <v>134</v>
       </c>
       <c r="F54" s="3">
         <v>1</v>
@@ -2241,511 +2266,445 @@
       <c r="G54" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H54" s="8" t="s">
-        <v>219</v>
+      <c r="H54" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>223</v>
+        <v>137</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>214</v>
+        <v>136</v>
       </c>
       <c r="F55" s="3">
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>219</v>
+        <v>205</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="F56" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="F58" s="3">
         <v>1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>219</v>
+        <v>41</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="F59" s="3">
         <v>1</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="F60" s="3">
         <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="F61" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G61" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F62" s="3">
-        <v>1</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="F63" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>160</v>
+        <v>44</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="F64" s="3">
         <v>1</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="F65" s="3">
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="H65" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="F66" s="3">
         <v>1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>220</v>
+        <v>159</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="F67" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="F69" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="F70" s="3">
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="F71" s="3">
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="F72" s="3">
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
-      <c r="C73" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D73" s="3" t="s">
+      <c r="C73" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <f>ROUND(44/66*100,0)</f>
         <v>67</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F73" s="3">
-        <v>1</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H73" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E75" s="5"/>
-      <c r="F75" s="3">
-        <v>1</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F76" s="3">
-        <v>1</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F77" s="3">
-        <v>1</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F78" s="3">
-        <v>1</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="F79" s="3">
-        <v>1</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F80" s="3">
-        <v>1</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>57</v>
+      <c r="J79" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C29 C68:C1048576 C1:C25 C32:C64" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27:C28 C62:C1048576 C31:C58 C1:C24" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
       <formula1>25</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E80 E82:E1048576 I79" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">
       <formula1>40</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update BOM EL, ajout images
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
+++ b/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\STUF2019\CR - Cost Report\BOM\EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD993B1-5E57-4174-A15F-8F0F9601E334}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1675EAD1-5D45-4B29-9C23-A73D04EAAD86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="660" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="210">
   <si>
     <t>System</t>
   </si>
@@ -304,15 +304,9 @@
     <t>suspension travel sensor</t>
   </si>
   <si>
-    <t>brake pressure sensor</t>
-  </si>
-  <si>
     <t>Lambda sensor</t>
   </si>
   <si>
-    <t>Fuel pressure sensor</t>
-  </si>
-  <si>
     <t>front harness</t>
   </si>
   <si>
@@ -322,15 +316,6 @@
     <t>paddle</t>
   </si>
   <si>
-    <t>Oil pressure sensor</t>
-  </si>
-  <si>
-    <t>Air pressure sensor</t>
-  </si>
-  <si>
-    <t>Air temp sensor</t>
-  </si>
-  <si>
     <t>Water temp sensor</t>
   </si>
   <si>
@@ -370,24 +355,12 @@
     <t>EL_02014</t>
   </si>
   <si>
-    <t>EL_02015</t>
-  </si>
-  <si>
-    <t>EL_02016</t>
-  </si>
-  <si>
-    <t>EL_02017</t>
-  </si>
-  <si>
     <t>on each four suspensions</t>
   </si>
   <si>
     <t>on each four wheels, Hall effect</t>
   </si>
   <si>
-    <t>pressure of rear and front brake sys.</t>
-  </si>
-  <si>
     <t>placed on the exhauste</t>
   </si>
   <si>
@@ -643,9 +616,6 @@
     <t>EL_04008</t>
   </si>
   <si>
-    <t>8STA01497P, Power and DATA</t>
-  </si>
-  <si>
     <t>8STA61497S, Power and DATA</t>
   </si>
   <si>
@@ -698,6 +668,24 @@
   </si>
   <si>
     <t>control the Dashboard and sensors</t>
+  </si>
+  <si>
+    <t>pressure sensors</t>
+  </si>
+  <si>
+    <t>Air temp and pressure  sensor</t>
+  </si>
+  <si>
+    <t>pressure of brake sys., fuel, oil</t>
+  </si>
+  <si>
+    <t>BSPD Box</t>
+  </si>
+  <si>
+    <t>EL_06006</t>
+  </si>
+  <si>
+    <t>8STA01497P&amp;S, Power and DATA</t>
   </si>
 </sst>
 </file>
@@ -1125,11 +1113,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1126,7 @@
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" style="8" customWidth="1"/>
@@ -1167,7 +1155,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1205,7 +1193,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1218,7 +1206,7 @@
         <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -1227,7 +1215,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1240,7 +1228,7 @@
         <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F5" s="3">
         <v>4</v>
@@ -1249,7 +1237,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1262,7 +1250,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -1271,7 +1259,7 @@
         <v>14</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1293,7 +1281,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1315,7 +1303,7 @@
         <v>73</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1337,20 +1325,20 @@
         <v>74</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -1359,20 +1347,20 @@
         <v>75</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -1381,20 +1369,20 @@
         <v>76</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
@@ -1402,19 +1390,21 @@
       <c r="G12" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -1423,7 +1413,7 @@
         <v>79</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1446,13 +1436,13 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -1461,20 +1451,20 @@
         <v>17</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1494,7 +1484,7 @@
         <v>65</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F17" s="3">
         <v>4</v>
@@ -1502,7 +1492,9 @@
       <c r="G17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
@@ -1514,7 +1506,7 @@
         <v>65</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F18" s="3">
         <v>4</v>
@@ -1522,19 +1514,21 @@
       <c r="G18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -1548,59 +1542,63 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>82</v>
+        <v>204</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>109</v>
+        <v>206</v>
       </c>
       <c r="F20" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H21" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="H22" s="3"/>
     </row>
@@ -1608,61 +1606,63 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="H24" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>170</v>
+        <v>102</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H25" s="3"/>
     </row>
@@ -1670,19 +1670,19 @@
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H26" s="3"/>
     </row>
@@ -1690,19 +1690,19 @@
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H27" s="3"/>
     </row>
@@ -1710,59 +1710,57 @@
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="F28" s="3">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F29" s="3">
-        <v>1</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H29" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="H30" s="3"/>
     </row>
@@ -1770,941 +1768,913 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>201</v>
+        <v>117</v>
       </c>
       <c r="F31" s="3">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="4"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="F33" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
       <c r="F34" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="F35" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>189</v>
+        <v>30</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F36" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="F37" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="F38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>204</v>
+        <v>163</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>150</v>
+        <v>198</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F41" s="3">
-        <v>1</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>189</v>
-      </c>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F42" s="3">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>124</v>
+        <v>31</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>208</v>
+        <v>57</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="F43" s="3">
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>125</v>
+        <v>32</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H44" s="4"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F44" s="3">
+        <v>2</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>192</v>
+        <v>126</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="F47" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>130</v>
+        <v>184</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>135</v>
+        <v>176</v>
       </c>
       <c r="F48" s="3">
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H48" s="3"/>
+        <v>153</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E49" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="F49" s="3">
-        <v>1</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="H49" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F50" s="3">
-        <v>1</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>189</v>
-      </c>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>193</v>
+        <v>124</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="F51" s="3">
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>162</v>
+        <v>38</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="F52" s="3">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H53" s="4"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F53" s="3">
+        <v>3</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="F54" s="3">
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F55" s="3">
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>205</v>
+        <v>41</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="F56" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="F57" s="3">
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
       <c r="F58" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="F59" s="3">
-        <v>1</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>189</v>
-      </c>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="F60" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H60" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="F61" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H62" s="4"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F63" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F64" s="3">
         <v>1</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="E65" s="3"/>
       <c r="F65" s="3">
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>46</v>
+        <v>208</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F66" s="3">
-        <v>1</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>189</v>
-      </c>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H66" s="4"/>
     </row>
     <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F67" s="3">
         <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H68" s="4"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F69" s="3">
         <v>1</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>189</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="H69" s="3"/>
     </row>
     <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="F70" s="3">
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H70" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
-      <c r="C71" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>187</v>
+      <c r="C71" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="F71" s="3">
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H71" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>178</v>
+        <v>105</v>
       </c>
       <c r="F72" s="3">
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="F73" s="3">
-        <v>1</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H73" s="3"/>
-    </row>
-    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F74" s="3">
-        <v>1</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I79">
-        <f>ROUND(44/66*100,0)</f>
-        <v>67</v>
-      </c>
-      <c r="J79" t="s">
-        <v>212</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <f>ROUND(56/64*100,0)</f>
+        <v>88</v>
+      </c>
+      <c r="J77" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27:C28 C62:C1048576 C31:C58 C1:C24" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 C28:C55 C1:C23 C59:C1048576" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
       <formula1>25</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E80 E82:E1048576 I79" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E80:E1048576 I77 E1:E78" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">
       <formula1>40</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
BOM EL dernières img, verif nom+taille img
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
+++ b/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\STUF2019\CR - Cost Report\BOM\EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1675EAD1-5D45-4B29-9C23-A73D04EAAD86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9C1F0A-0D86-4BCD-A1DC-13AC13E83C82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="213">
   <si>
     <t>System</t>
   </si>
@@ -247,9 +247,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>over the front hoop</t>
-  </si>
-  <si>
     <t>LED Bar</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
     <t>EL_01011</t>
   </si>
   <si>
-    <t>EL_01012</t>
-  </si>
-  <si>
     <t>wheel speed sensor</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
     <t>connector rear board 1</t>
   </si>
   <si>
-    <t>connector rear board 2</t>
-  </si>
-  <si>
     <t>connector front board 1</t>
   </si>
   <si>
@@ -406,9 +397,6 @@
     <t>EL_03010</t>
   </si>
   <si>
-    <t>EL_03011</t>
-  </si>
-  <si>
     <t>link fr. , servo motor, sensors, bat.</t>
   </si>
   <si>
@@ -442,18 +430,12 @@
     <t>in the Fuse box</t>
   </si>
   <si>
-    <t>Brake light Fuse 2A</t>
-  </si>
-  <si>
     <t>EL_05007</t>
   </si>
   <si>
     <t>EL_05008</t>
   </si>
   <si>
-    <t>Dashboard kill Switch</t>
-  </si>
-  <si>
     <t>Master switch</t>
   </si>
   <si>
@@ -472,9 +454,6 @@
     <t>BSPD</t>
   </si>
   <si>
-    <t>BOTS</t>
-  </si>
-  <si>
     <t>data logger</t>
   </si>
   <si>
@@ -538,9 +517,6 @@
     <t>display water temp. Or Batt. Voltage</t>
   </si>
   <si>
-    <t>connector for MK3</t>
-  </si>
-  <si>
     <t>to the DTA</t>
   </si>
   <si>
@@ -556,12 +532,6 @@
     <t>on both sides of the main hoop</t>
   </si>
   <si>
-    <t>on the Dashboard</t>
-  </si>
-  <si>
-    <t>behind the brake pedale</t>
-  </si>
-  <si>
     <t>protecting plastic case</t>
   </si>
   <si>
@@ -616,9 +586,6 @@
     <t>EL_04008</t>
   </si>
   <si>
-    <t>8STA61497S, Power and DATA</t>
-  </si>
-  <si>
     <t>Servo motor Fuse 15A</t>
   </si>
   <si>
@@ -631,9 +598,6 @@
     <t>battery connector</t>
   </si>
   <si>
-    <t>8STA10235S&amp;P, to the harness (fr./re.)</t>
-  </si>
-  <si>
     <t>8STA71828S&amp;P, sensors and Power</t>
   </si>
   <si>
@@ -682,10 +646,55 @@
     <t>BSPD Box</t>
   </si>
   <si>
-    <t>EL_06006</t>
-  </si>
-  <si>
     <t>8STA01497P&amp;S, Power and DATA</t>
+  </si>
+  <si>
+    <t>connectors for MK3</t>
+  </si>
+  <si>
+    <t>EL_01003</t>
+  </si>
+  <si>
+    <t>24mm kill Switch</t>
+  </si>
+  <si>
+    <t>Dashboard and BOTS</t>
+  </si>
+  <si>
+    <t>Brake light Fuse 3A</t>
+  </si>
+  <si>
+    <t>lambda connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to the harness (fr./re.)</t>
+  </si>
+  <si>
+    <t>EL_02015</t>
+  </si>
+  <si>
+    <t>standard automobile connector</t>
+  </si>
+  <si>
+    <t>3 pin connector</t>
+  </si>
+  <si>
+    <t>EL_02016</t>
+  </si>
+  <si>
+    <t>EL_02017</t>
+  </si>
+  <si>
+    <t>2 pin connector</t>
+  </si>
+  <si>
+    <t>connector to the injector</t>
+  </si>
+  <si>
+    <t>EL_02018</t>
+  </si>
+  <si>
+    <t>inside the front hoop</t>
   </si>
 </sst>
 </file>
@@ -807,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -820,9 +829,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1113,11 +1119,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1135,7 @@
     <col min="5" max="5" width="35.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1154,8 +1160,8 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>179</v>
+      <c r="H1" s="5" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1184,7 +1190,7 @@
         <v>62</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>63</v>
+        <v>212</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -1192,21 +1198,21 @@
       <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>180</v>
+      <c r="H3" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -1214,206 +1220,206 @@
       <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>180</v>
+      <c r="H4" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F5" s="3">
         <v>4</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>180</v>
+        <v>198</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>180</v>
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>180</v>
+        <v>14</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="3">
         <v>2</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>180</v>
+        <v>15</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="3">
         <v>2</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>180</v>
+        <v>72</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>180</v>
+        <v>73</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>180</v>
+        <v>74</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>180</v>
+        <v>75</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>180</v>
+        <v>77</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1436,13 +1442,13 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -1451,20 +1457,20 @@
         <v>17</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1472,19 +1478,21 @@
       <c r="G16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F17" s="3">
         <v>4</v>
@@ -1493,20 +1501,20 @@
         <v>19</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F18" s="3">
         <v>4</v>
@@ -1515,20 +1523,20 @@
         <v>20</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -1536,19 +1544,21 @@
       <c r="G19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="F20" s="3">
         <v>4</v>
@@ -1557,1124 +1567,1180 @@
         <v>22</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H22" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H26" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H27" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="F28" s="3">
         <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="4"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>83</v>
+        <v>206</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>118</v>
+        <v>205</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" s="3"/>
+        <v>207</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>84</v>
+        <v>209</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>26</v>
+        <v>208</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="F32" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>27</v>
+        <v>211</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F33" s="3">
-        <v>4</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>209</v>
+        <v>114</v>
       </c>
       <c r="F34" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
       <c r="F35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="F37" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="F38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H41" s="4"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="F42" s="3">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F43" s="3">
-        <v>1</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F44" s="3">
-        <v>2</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>180</v>
-      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F47" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>184</v>
+        <v>117</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>176</v>
+        <v>122</v>
       </c>
       <c r="F48" s="3">
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>153</v>
+        <v>34</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="F49" s="3">
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H50" s="4"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="F51" s="3">
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="F52" s="3">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="F53" s="3">
-        <v>3</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>189</v>
+        <v>121</v>
       </c>
       <c r="F54" s="3">
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="F55" s="3">
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>41</v>
+        <v>183</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F56" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F57" s="3">
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>181</v>
+        <v>119</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="F58" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H59" s="4"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F60" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F61" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F62" s="3">
-        <v>1</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="F63" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="F64" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>207</v>
+        <v>131</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E65" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="F65" s="3">
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>208</v>
+        <v>46</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H66" s="4"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F66" s="3">
+        <v>1</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>148</v>
+        <v>195</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>168</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E67" s="3"/>
       <c r="F67" s="3">
         <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F68" s="3">
-        <v>1</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H68" s="4"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="F69" s="3">
         <v>1</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H69" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="F70" s="3">
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
-      <c r="C71" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>201</v>
+      <c r="C71" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="F71" s="3">
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="F72" s="3">
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1</v>
+      </c>
+      <c r="G74" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H72" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I77">
+      <c r="H74" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I79">
         <f>ROUND(56/64*100,0)</f>
         <v>88</v>
       </c>
-      <c r="J77" t="s">
-        <v>202</v>
+      <c r="J79" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 C28:C55 C1:C23 C59:C1048576" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 C1:C23 C62:C1048576 C28:C58" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
       <formula1>25</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E80:E1048576 I77 E1:E78" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E82:E1048576 I79 E1:E80" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">
       <formula1>40</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
un max de truc
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
+++ b/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\STUF2019\CR - Cost Report\BOM\EL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\CR - Cost Report\BOM\EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9C1F0A-0D86-4BCD-A1DC-13AC13E83C82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20783CFD-8293-47D8-A9C3-A4EEA9677786}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="223">
   <si>
     <t>System</t>
   </si>
@@ -695,6 +694,36 @@
   </si>
   <si>
     <t>inside the front hoop</t>
+  </si>
+  <si>
+    <t>Plutôt booster connector ( ou Anderson connector pour son vrai nom)</t>
+  </si>
+  <si>
+    <t>c'était clairement intégré dans le moteur je sais pas si on peut dire que c'est une pièce à part</t>
+  </si>
+  <si>
+    <t>pareil que au dessus</t>
+  </si>
+  <si>
+    <t>de même</t>
+  </si>
+  <si>
+    <t>je sais pas de quoi tu parle..</t>
+  </si>
+  <si>
+    <t>il y a deux connecteur pour le dta, un de puissance un pour sensor</t>
+  </si>
+  <si>
+    <t>3 connecteurs sur la boite avant</t>
+  </si>
+  <si>
+    <t>2 connecteurs sur la boite arrière</t>
+  </si>
+  <si>
+    <t>à termes deux connecteur sur la pare feu</t>
+  </si>
+  <si>
+    <t>1 connecteur BSPD</t>
   </si>
 </sst>
 </file>
@@ -816,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -838,6 +867,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1122,8 +1154,8 @@
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,6 +1168,7 @@
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1482,7 +1515,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
@@ -1504,7 +1537,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
@@ -1526,7 +1559,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
@@ -1548,7 +1581,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
@@ -1570,7 +1603,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
@@ -1592,7 +1625,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -1613,8 +1646,11 @@
       <c r="H22" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
@@ -1636,7 +1672,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
@@ -1658,7 +1694,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
@@ -1679,8 +1715,11 @@
       <c r="H25" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -1701,8 +1740,11 @@
       <c r="H26" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
@@ -1724,7 +1766,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
@@ -1745,8 +1787,11 @@
       <c r="H28" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
@@ -1768,7 +1813,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
@@ -1790,7 +1835,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
@@ -1812,7 +1857,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
@@ -1834,7 +1879,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
@@ -1850,7 +1895,7 @@
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
@@ -1872,7 +1917,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
@@ -1894,7 +1939,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
@@ -1915,8 +1960,11 @@
       <c r="H36" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I36" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
@@ -1937,8 +1985,11 @@
       <c r="H37" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I37" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -1959,8 +2010,11 @@
       <c r="H38" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I38" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
@@ -1981,8 +2035,11 @@
       <c r="H39" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I39" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
@@ -2004,7 +2061,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
@@ -2026,7 +2083,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
@@ -2047,8 +2104,11 @@
       <c r="H42" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I42" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
@@ -2070,7 +2130,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -2086,7 +2146,7 @@
       </c>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
@@ -2108,7 +2168,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
@@ -2130,7 +2190,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
@@ -2152,7 +2212,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
@@ -2174,7 +2234,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
@@ -2196,7 +2256,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
@@ -2218,7 +2278,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
@@ -2239,8 +2299,11 @@
       <c r="H51" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I51" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
@@ -2262,7 +2325,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>7</v>
       </c>
@@ -2278,7 +2341,7 @@
       </c>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
@@ -2300,7 +2363,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
@@ -2322,7 +2385,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
@@ -2344,7 +2407,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
@@ -2366,7 +2429,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
@@ -2388,7 +2451,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
@@ -2410,7 +2473,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
@@ -2432,7 +2495,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
@@ -2454,7 +2517,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
@@ -2470,7 +2533,7 @@
       </c>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
@@ -2492,7 +2555,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">

</xml_diff>

<commit_message>
Le cost c'est fun
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
+++ b/CR - Cost Report/BOM/EL/ELA0100_to_ELA0700.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\CR - Cost Report\BOM\EL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20783CFD-8293-47D8-A9C3-A4EEA9677786}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,9 +86,6 @@
     <t>Sensors</t>
   </si>
   <si>
-    <t>EL_A0001</t>
-  </si>
-  <si>
     <t>EL_01001</t>
   </si>
   <si>
@@ -105,9 +101,6 @@
     <t>EL_01006</t>
   </si>
   <si>
-    <t>EL_A0002</t>
-  </si>
-  <si>
     <t>EL_02001</t>
   </si>
   <si>
@@ -126,12 +119,6 @@
     <t>EL_02006</t>
   </si>
   <si>
-    <t>EL_A0003</t>
-  </si>
-  <si>
-    <t>EL_A0004</t>
-  </si>
-  <si>
     <t>EL_03001</t>
   </si>
   <si>
@@ -168,9 +155,6 @@
     <t>EL_04006</t>
   </si>
   <si>
-    <t>EL_A0005</t>
-  </si>
-  <si>
     <t>EL_05001</t>
   </si>
   <si>
@@ -186,9 +170,6 @@
     <t>EL_05006</t>
   </si>
   <si>
-    <t>EL_A0006</t>
-  </si>
-  <si>
     <t>EL_06001</t>
   </si>
   <si>
@@ -204,9 +185,6 @@
     <t>EL_06005</t>
   </si>
   <si>
-    <t>EL_A0007</t>
-  </si>
-  <si>
     <t>EL_07001</t>
   </si>
   <si>
@@ -724,12 +702,33 @@
   </si>
   <si>
     <t>1 connecteur BSPD</t>
+  </si>
+  <si>
+    <t>EL_A0100</t>
+  </si>
+  <si>
+    <t>EL_A0200</t>
+  </si>
+  <si>
+    <t>EL_A0300</t>
+  </si>
+  <si>
+    <t>EL_A0400</t>
+  </si>
+  <si>
+    <t>EL_A0500</t>
+  </si>
+  <si>
+    <t>EL_A0600</t>
+  </si>
+  <si>
+    <t>EL_A0700</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1150,28 +1149,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="58.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1194,10 +1193,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1209,253 +1208,253 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>10</v>
+        <v>216</v>
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F5" s="3">
         <v>4</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F8" s="3">
         <v>2</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F9" s="3">
         <v>2</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1467,1343 +1466,1343 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F17" s="3">
         <v>4</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F18" s="3">
         <v>4</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F20" s="3">
         <v>4</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="H25" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F28" s="3">
         <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F32" s="3">
         <v>4</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
-        <v>23</v>
+        <v>218</v>
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F37" s="3">
         <v>4</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F38" s="3">
         <v>2</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F41" s="3">
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F42" s="3">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F43" s="3">
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4" t="s">
-        <v>24</v>
+        <v>219</v>
       </c>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F47" s="3">
         <v>2</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F48" s="3">
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F49" s="3">
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F50" s="3">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F51" s="3">
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F52" s="3">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4" t="s">
-        <v>37</v>
+        <v>220</v>
       </c>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F54" s="3">
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F55" s="3">
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F56" s="3">
         <v>3</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F57" s="3">
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F58" s="3">
         <v>1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F59" s="3">
         <v>1</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F60" s="3">
         <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F61" s="3">
         <v>4</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4" t="s">
-        <v>43</v>
+        <v>221</v>
       </c>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F63" s="3">
         <v>2</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F64" s="3">
         <v>2</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F65" s="3">
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F66" s="3">
         <v>1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3">
         <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4" t="s">
-        <v>49</v>
+        <v>222</v>
       </c>
       <c r="H68" s="4"/>
     </row>
-    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F69" s="3">
         <v>1</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F70" s="3">
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F71" s="3">
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F72" s="3">
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F73" s="3">
         <v>1</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F74" s="3">
         <v>1</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I79">
         <f>ROUND(56/64*100,0)</f>
         <v>88</v>
       </c>
       <c r="J79" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 C1:C23 C62:C1048576 C28:C58" xr:uid="{6984A51B-6EDF-4CEC-BE77-A77BD9FB97B6}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 C1:C23 C62:C1048576 C28:C58">
       <formula1>25</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E82:E1048576 I79 E1:E80" xr:uid="{7AA29FA9-BB55-4304-98F2-EF042CBAC3ED}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E82:E1048576 I79 E1:E80">
       <formula1>40</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>